<commit_message>
change image location ,update bug list excel.
</commit_message>
<xml_diff>
--- a/iphone/bugList.xlsx
+++ b/iphone/bugList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36540" yWindow="-280" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -276,6 +276,14 @@
   </si>
   <si>
     <t>按钮尺寸已经改大</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示是根据用户登陆的app store所在的地区显示的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>closed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -385,6 +393,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="31">
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -400,22 +424,6 @@
     <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -746,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -1007,7 +1015,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="34">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
@@ -1021,10 +1029,13 @@
         <v>41346</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:7">

</xml_diff>

<commit_message>
added a device id and updated Development Provisioning Profile , updated bug status
</commit_message>
<xml_diff>
--- a/iphone/bugList.xlsx
+++ b/iphone/bugList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
   <si>
     <t>描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -150,10 +150,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>点击store中的"tell your twitter friends",提示去settings输入twitter的账号，完成后却没有发消息去twitter的界面。这是在5.0的模拟器上发现的。6.0的模拟器也有这个问题。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>medium</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -194,10 +190,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>fixed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>closed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -214,10 +206,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>目前是改为发送news的动作实际进行后才加币，不过尚不能控制等到实际发送成功再加币。目前在模拟器6.0上和ipad以及iphone好使，但touch的ios6.1.2上按钮一点就出问题。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>app的store即使在美国那边也显示人民币</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -271,14 +259,6 @@
   </si>
   <si>
     <t>closed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>下一步是消息内容确认</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -313,6 +293,16 @@
   </si>
   <si>
     <t>点击被lock的package，提示需要去store购买的对话框上的Ok改为buy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击store中的"tell your twitter friends",提示去settings输入twitter的账号，完成后却没有发消息去twitter的界面。这是在5.0的模拟器上发现的。6.0的模拟器也有这个问题。
+另外有问题是在Ask Friends中点击facebook或twitter的按钮也有类似问题。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目前是改为发送news的动作实际进行后才加币，不过尚不能控制等到实际发送成功再加币。目前在模拟器6.0上和ipad以及iphone4s好使，但touch的ios6.1.2上按钮一点就出问题。又发现在iphone5上一点app就崩掉。
+后来的解决方式是加了对于nil的判断，nil一般是由于device中没有已经登录的account导致的，如果出现nil会弹出消息框提示先去登录facebook或twitter的account。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -379,8 +369,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -433,7 +427,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="47">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -455,6 +449,8 @@
     <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -476,6 +472,8 @@
     <cellStyle name="访问过的超链接" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -807,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -881,13 +879,13 @@
         <v>41342</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="37" customHeight="1">
@@ -910,9 +908,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="85">
+    <row r="5" spans="1:7" ht="187">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -924,13 +922,13 @@
         <v>41345</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="51">
@@ -958,7 +956,7 @@
     </row>
     <row r="7" spans="1:7" ht="187">
       <c r="A7" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
@@ -981,7 +979,7 @@
     </row>
     <row r="8" spans="1:7" ht="34">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>22</v>
@@ -999,113 +997,113 @@
         <v>31</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="34">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2">
         <v>41345</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="34">
       <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D10" s="2">
         <v>41345</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="51">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11" s="2">
         <v>41345</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="34">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D12" s="2">
         <v>41346</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="D13" s="2">
         <v>41346</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>28</v>
@@ -1113,53 +1111,50 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D14" s="2">
         <v>41346</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="15" spans="1:7" ht="34">
       <c r="A15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D15" s="2">
         <v>41346</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D16" s="2">
         <v>41352</v>
@@ -1170,13 +1165,13 @@
     </row>
     <row r="17" spans="1:5" ht="34">
       <c r="A17" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D17" s="2">
         <v>41352</v>
@@ -1187,13 +1182,13 @@
     </row>
     <row r="18" spans="1:5" ht="34">
       <c r="A18" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D18" s="2">
         <v>41352</v>

</xml_diff>